<commit_message>
update in the sequence diagram
</commit_message>
<xml_diff>
--- a/Fase_II/Use Cases/Edita receita.xlsx
+++ b/Fase_II/Use Cases/Edita receita.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nuno\Desktop\Li4---Sweetron\Fase_II\Use Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{31F9CA2E-772A-422D-B5E0-603863FD730E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F5C8D8-54DC-43AF-9CFD-76DC7DFE7E48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="84" yWindow="456" windowWidth="25440" windowHeight="14724" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
@@ -82,10 +82,10 @@
     <t>7. Notifica que a receita foi alterada com sucesso</t>
   </si>
   <si>
-    <t>Exceção      [Cancela edição]     (passo 5)</t>
-  </si>
-  <si>
     <t>5.1 Cancela edição</t>
+  </si>
+  <si>
+    <t>Exceção      [Cancela edição]     (passo 4)</t>
   </si>
 </sst>
 </file>
@@ -360,26 +360,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -399,6 +379,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -408,7 +397,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,7 +726,7 @@
   <dimension ref="B1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="B14" sqref="B14:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -742,124 +742,124 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="11"/>
+      <c r="D2" s="28"/>
     </row>
     <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="11"/>
+      <c r="D3" s="28"/>
     </row>
     <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="11"/>
+      <c r="D4" s="28"/>
     </row>
     <row r="5" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="13"/>
+      <c r="D5" s="30"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="11" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="36" x14ac:dyDescent="0.35">
-      <c r="B7" s="16"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="24"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="2:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="B8" s="16"/>
-      <c r="C8" s="25"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="17"/>
       <c r="D8" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="36" x14ac:dyDescent="0.35">
-      <c r="B9" s="16"/>
-      <c r="C9" s="26"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="18"/>
       <c r="D9" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="14"/>
-      <c r="C10" s="21" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="22"/>
+      <c r="D10" s="14"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="14"/>
-      <c r="C11" s="21" t="s">
+      <c r="B11" s="22"/>
+      <c r="C11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="22"/>
+      <c r="D11" s="14"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="14"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="22" t="s">
+      <c r="B12" s="22"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="15"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="23" t="s">
+      <c r="B13" s="23"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="20"/>
+      <c r="D14" s="12"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="28"/>
+      <c r="B15" s="25"/>
       <c r="C15" s="8"/>
       <c r="D15" s="5"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="28"/>
+      <c r="B16" s="25"/>
       <c r="C16" s="8"/>
       <c r="D16" s="5"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="28"/>
+      <c r="B17" s="25"/>
       <c r="C17" s="8"/>
       <c r="D17" s="5"/>
     </row>
     <row r="18" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="29"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="9"/>
       <c r="D18" s="6"/>
     </row>

</xml_diff>